<commit_message>
modify paper score model
</commit_message>
<xml_diff>
--- a/server/shell/paper-score.xlsx
+++ b/server/shell/paper-score.xlsx
@@ -16,12 +16,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -30,15 +30,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -52,9 +46,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -68,7 +76,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -84,7 +92,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -98,9 +106,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -114,9 +137,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,36 +152,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -167,17 +166,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -190,13 +183,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -208,169 +363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +396,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -412,7 +405,37 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -428,21 +451,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -466,165 +474,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -635,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -953,15 +946,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1">
         <v>15</v>
       </c>
@@ -980,8 +973,15 @@
       <c r="F1" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1">
+        <f>SUM(A1:F1)</f>
+        <v>67</v>
+      </c>
+      <c r="H1">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>15</v>
       </c>
@@ -1000,8 +1000,15 @@
       <c r="F2" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <f t="shared" ref="G2:G36" si="0">SUM(A2:F2)</f>
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>12</v>
       </c>
@@ -1020,8 +1027,15 @@
       <c r="F3" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="H3">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -1040,8 +1054,15 @@
       <c r="F4" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="H4">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>14</v>
       </c>
@@ -1060,8 +1081,15 @@
       <c r="F5" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="H5">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>13</v>
       </c>
@@ -1080,8 +1108,15 @@
       <c r="F6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="H6">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>13</v>
       </c>
@@ -1100,8 +1135,15 @@
       <c r="F7" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="H7">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>14</v>
       </c>
@@ -1120,8 +1162,15 @@
       <c r="F8" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="H8">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>12</v>
       </c>
@@ -1140,8 +1189,15 @@
       <c r="F9" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="H9">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1160,8 +1216,15 @@
       <c r="F10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H10">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1180,8 +1243,15 @@
       <c r="F11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1200,8 +1270,15 @@
       <c r="F12" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="H12">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -1220,8 +1297,15 @@
       <c r="F13" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="H13">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -1240,8 +1324,15 @@
       <c r="F14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="H14">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1260,8 +1351,15 @@
       <c r="F15" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="H15">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1280,8 +1378,15 @@
       <c r="F16" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="H16">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -1300,8 +1405,15 @@
       <c r="F17" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="H17">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>13</v>
       </c>
@@ -1320,8 +1432,15 @@
       <c r="F18" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="H18">
+        <v>1501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>9</v>
       </c>
@@ -1340,8 +1459,15 @@
       <c r="F19" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="H19">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>12</v>
       </c>
@@ -1360,8 +1486,15 @@
       <c r="F20" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="H20">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>12</v>
       </c>
@@ -1380,8 +1513,15 @@
       <c r="F21" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="H21">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -1400,8 +1540,15 @@
       <c r="F22" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="H22">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>15</v>
       </c>
@@ -1420,8 +1567,15 @@
       <c r="F23" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="H23">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>15</v>
       </c>
@@ -1440,8 +1594,15 @@
       <c r="F24" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="H24">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>15</v>
       </c>
@@ -1460,8 +1621,15 @@
       <c r="F25" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="H25">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>11</v>
       </c>
@@ -1480,8 +1648,15 @@
       <c r="F26" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="H26">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>12</v>
       </c>
@@ -1500,8 +1675,15 @@
       <c r="F27" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H27">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>15</v>
       </c>
@@ -1520,8 +1702,15 @@
       <c r="F28" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H28">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>15</v>
       </c>
@@ -1540,8 +1729,15 @@
       <c r="F29" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H29">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>15</v>
       </c>
@@ -1560,8 +1756,15 @@
       <c r="F30" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="H30">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>14</v>
       </c>
@@ -1580,8 +1783,15 @@
       <c r="F31" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H31">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>15</v>
       </c>
@@ -1600,8 +1810,15 @@
       <c r="F32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="H32">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>15</v>
       </c>
@@ -1620,8 +1837,15 @@
       <c r="F33" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="H33">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>15</v>
       </c>
@@ -1640,8 +1864,15 @@
       <c r="F34" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="H34">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>15</v>
       </c>
@@ -1660,8 +1891,15 @@
       <c r="F35" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="H35">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>6</v>
       </c>
@@ -1679,6 +1917,13 @@
       </c>
       <c r="F36" s="1">
         <v>25</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H36">
+        <v>1502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>